<commit_message>
Update the 720, 40C and 120 offenses' categories.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesArkansas.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesArkansas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiqiwei/git/nibrsSpringBoot2/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0A56BD-9740-8D49-AAF4-F6EB4BD1C749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A031F8D6-88A3-8242-A85F-20BF933C17DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="2800" windowWidth="20480" windowHeight="12400" tabRatio="705" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32640" yWindow="2800" windowWidth="20480" windowHeight="12400" tabRatio="705" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -21635,8 +21635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58:E58"/>
+    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -21824,7 +21824,7 @@
         <v>530</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
@@ -23410,13 +23410,13 @@
         <v>632</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>610</v>
+        <v>521</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>614</v>
+        <v>632</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>579</v>
@@ -23468,7 +23468,7 @@
         <v>637</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>610</v>
+        <v>521</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>168</v>
@@ -25058,7 +25058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>